<commit_message>
added csv to csv test case
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400AF054-24AD-412F-946F-BDBF096555C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4712541-F4CE-45E9-992A-1C95582C386A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Sno.</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>execute</t>
+  </si>
+  <si>
+    <t>testcase27_csv_csv_bigdata_match</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,10 +1034,19 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f>_xlfn.CONCAT("/app/test/testcases/",B28,".xlsx")</f>
+        <v>/app/test/testcases/testcase27_csv_csv_bigdata_match.xlsx</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -1104,7 +1116,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D28" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
sample demo ready code
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E59F27-5D1F-4A0C-A119-9B54AFAA1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD895E85-0639-4543-86C2-21878A49FA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Sno.</t>
   </si>
@@ -169,13 +169,22 @@
   </si>
   <si>
     <t>DBTablesDemo</t>
+  </si>
+  <si>
+    <t>testcase28_csv_sample1_csv_sample2</t>
+  </si>
+  <si>
+    <t>testcase29_csv_sample2_csv_sample3</t>
+  </si>
+  <si>
+    <t>testcase30_csv_sample1_csv_sample3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +196,12 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,7 +564,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,22 +1064,49 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <f>_xlfn.CONCAT("/app/test/testcases/",B29,".xlsx")</f>
+        <v>/app/test/testcases/testcase28_csv_sample1_csv_sample2.xlsx</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f t="shared" ref="C30:C31" si="1">_xlfn.CONCAT("/app/test/testcases/",B30,".xlsx")</f>
+        <v>/app/test/testcases/testcase29_csv_sample2_csv_sample3.xlsx</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>/app/test/testcases/testcase30_csv_sample1_csv_sample3.xlsx</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
@@ -1115,8 +1157,9 @@
       <c r="D39" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D28" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
clean up of atf code
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD895E85-0639-4543-86C2-21878A49FA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B01F3-78F0-46D7-A79A-A7174940E991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Sno.</t>
   </si>
@@ -171,13 +171,7 @@
     <t>DBTablesDemo</t>
   </si>
   <si>
-    <t>testcase28_csv_sample1_csv_sample2</t>
-  </si>
-  <si>
-    <t>testcase29_csv_sample2_csv_sample3</t>
-  </si>
-  <si>
-    <t>testcase30_csv_sample1_csv_sample3</t>
+    <t>testcase28_manual_sql_etltesting</t>
   </si>
 </sst>
 </file>
@@ -630,10 +624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,41 +1066,23 @@
       </c>
       <c r="C29" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B29,".xlsx")</f>
-        <v>/app/test/testcases/testcase28_csv_sample1_csv_sample2.xlsx</v>
+        <v>/app/test/testcases/testcase28_manual_sql_etltesting.xlsx</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="4" t="str">
-        <f t="shared" ref="C30:C31" si="1">_xlfn.CONCAT("/app/test/testcases/",B30,".xlsx")</f>
-        <v>/app/test/testcases/testcase29_csv_sample2_csv_sample3.xlsx</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>/app/test/testcases/testcase30_csv_sample1_csv_sample3.xlsx</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
@@ -1144,22 +1120,10 @@
       <c r="C37" s="4"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="6"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Manual SQL fixes, Demo Ready
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B01F3-78F0-46D7-A79A-A7174940E991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB71674-F617-4EAF-8500-E383917248EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Sno.</t>
   </si>
@@ -171,7 +171,10 @@
     <t>DBTablesDemo</t>
   </si>
   <si>
-    <t>testcase28_manual_sql_etltesting</t>
+    <t>testcase28_manual_sql_notifications</t>
+  </si>
+  <si>
+    <t>testcase29_manual_sql_fullname</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +922,7 @@
         <v>/app/test/testcases/testcase18_parquet_dbtable_match_likeobject.xlsx</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,7 +937,7 @@
         <v>/app/test/testcases/testcase19_oracle_mysql_match_manual.xlsx</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,7 +967,7 @@
         <v>/app/test/testcases/testcase21_mysql_csv_match.xlsx</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,17 +1069,26 @@
       </c>
       <c r="C29" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B29,".xlsx")</f>
-        <v>/app/test/testcases/testcase28_manual_sql_etltesting.xlsx</v>
+        <v>/app/test/testcases/testcase28_manual_sql_notifications.xlsx</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f>_xlfn.CONCAT("/app/test/testcases/",B30,".xlsx")</f>
+        <v>/app/test/testcases/testcase29_manual_sql_fullname.xlsx</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
@@ -1123,7 +1135,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30" xr:uid="{864DC9FE-D2BF-46C6-8674-EF3F47262FBF}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
BigData Match for 50 cols
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB5EA71-98F5-407D-A0A0-9CF32923AB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA62AC9B-C0D4-420E-9072-0502E04DC928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Sno.</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>testcase29_manual_sql_fullname</t>
+  </si>
+  <si>
+    <t>testcase30_csv_csv_3mill50cols_content</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1094,19 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <f>_xlfn.CONCAT("/app/test/testcases/",B31,".xlsx")</f>
+        <v>/app/test/testcases/testcase30_csv_csv_3mill50cols_content.xlsx</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>

</xml_diff>

<commit_message>
renaming pdf in output reports
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA62AC9B-C0D4-420E-9072-0502E04DC928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5908531D-1787-4E01-9DC5-252B216AA538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol" sheetId="1" r:id="rId1"/>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +925,7 @@
         <v>/app/test/testcases/testcase18_parquet_dbtable_match_likeobject.xlsx</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>/app/test/testcases/testcase19_oracle_mysql_match_manual.xlsx</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>/app/test/testcases/testcase21_mysql_csv_match.xlsx</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>/app/test/testcases/testcase28_manual_sql_notifications.xlsx</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>/app/test/testcases/testcase29_manual_sql_fullname.xlsx</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
content failure not fixed
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9893AD-373F-4F1E-A875-A7D9016C0102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2178DA7F-0DB4-4B8E-8D22-46E551003E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
         <v>test\\testcases\\testcase23_snowflake_snowflake_match.xlsx</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>test\\testcases\\testcase24_snowflake_snowflake_etljob.xlsx</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
demo ready on ubuntu
</commit_message>
<xml_diff>
--- a/test/testprotocol/testprotocol.xlsx
+++ b/test/testprotocol/testprotocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\QE_ATF\test\testprotocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Snowflake\QE_ATF\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B0A16F-45E4-46FD-9216-C4478BB6BFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF53B758-6C8F-4FC3-A0EA-DF6348DFC73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
         <v>test\testcases\testcase28_manual_sql_notifications.xlsx</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>